<commit_message>
Update at 21.09: 18:00
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gorbatova Svetlana\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G528\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70BFBBE0-9035-4D97-88A2-2BCB3B4D665C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9600"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="БИВТ-22-17" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'БИВТ-22-18'!$A$1:$B$26</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'БИВТ-22-20'!$A$1:$B$30</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,12 +30,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -42,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="102">
   <si>
     <t>ФИО</t>
   </si>
@@ -353,7 +351,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -985,11 +983,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1945,8 +1943,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B32">
-    <sortState ref="A2:B32">
+  <autoFilter ref="A1:B32" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B32">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
@@ -1956,11 +1954,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2048,7 +2046,9 @@
       <c r="A3" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="14"/>
+      <c r="B3" s="14" t="s">
+        <v>100</v>
+      </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -2155,8 +2155,8 @@
       <c r="B7" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>101</v>
+      <c r="C7" s="1">
+        <v>5</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -2170,7 +2170,7 @@
       <c r="M7" s="1"/>
       <c r="N7" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O7" s="3">
         <f t="shared" si="1"/>
@@ -2181,7 +2181,9 @@
       <c r="A8" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="14"/>
+      <c r="B8" s="14" t="s">
+        <v>100</v>
+      </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -2209,8 +2211,8 @@
       <c r="B9" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>101</v>
+      <c r="C9" s="1">
+        <v>5</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -2224,7 +2226,7 @@
       <c r="M9" s="1"/>
       <c r="N9" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O9" s="3">
         <f t="shared" si="1"/>
@@ -2317,7 +2319,9 @@
       <c r="B13" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -2477,7 +2481,9 @@
       <c r="B19" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="C19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -2504,8 +2510,8 @@
       <c r="B20" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>101</v>
+      <c r="C20" s="1">
+        <v>5</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -2519,7 +2525,7 @@
       <c r="M20" s="1"/>
       <c r="N20" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O20" s="3">
         <f t="shared" si="1"/>
@@ -2690,47 +2696,47 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C27">
-        <f>COUNT(#REF!)</f>
-        <v>0</v>
+        <f>COUNT(C2:C26)</f>
+        <v>3</v>
       </c>
       <c r="D27">
-        <f t="shared" ref="D27" si="2">COUNT(#REF!)</f>
+        <f t="shared" ref="D27:M27" si="2">COUNT(D2:D26)</f>
         <v>0</v>
       </c>
       <c r="E27">
-        <f t="shared" ref="E27" si="3">COUNT(#REF!)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F27">
-        <f t="shared" ref="F27" si="4">COUNT(#REF!)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G27">
-        <f t="shared" ref="G27" si="5">COUNT(#REF!)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H27">
-        <f t="shared" ref="H27" si="6">COUNT(#REF!)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I27">
-        <f t="shared" ref="I27" si="7">COUNT(#REF!)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J27">
-        <f t="shared" ref="J27" si="8">COUNT(#REF!)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K27">
-        <f t="shared" ref="K27" si="9">COUNT(#REF!)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L27">
-        <f t="shared" ref="L27" si="10">COUNT(#REF!)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M27">
-        <f t="shared" ref="M27" si="11">COUNT(#REF!)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N27" s="20"/>
@@ -2757,8 +2763,8 @@
       <c r="O32" s="20"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B26"/>
-  <sortState ref="A2:B26">
+  <autoFilter ref="A1:B26" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B26">
     <sortCondition ref="A1:A26"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2766,7 +2772,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3675,8 +3681,8 @@
       <c r="O32" s="20"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B30"/>
-  <sortState ref="A2:B30">
+  <autoFilter ref="A1:B30" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B30">
     <sortCondition ref="A1:A30"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>